<commit_message>
XLSX styles support for rows and columns, new features, updated Demo10
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -476,30 +476,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">

</xml_diff>

<commit_message>
Merge cells support in XLWorksheet::mergeCells & ::unmergeCells, XLCell::clear method added
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="General" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Worksheet name test" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="15" r:id="rId18"/>
     <sheet name="ChangeLog" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Containers" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Parameters" sheetId="4" state="visible" r:id="rId6"/>
@@ -21,6 +22,7 @@
     <sheet name="CommandVerification" sheetId="11" state="visible" r:id="rId13"/>
     <sheet name="Alarms" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="Algorithms" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet state="veryHidden" name="Sheet2" sheetId="14" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t xml:space="preserve">format version</t>
   </si>
@@ -69,6 +71,9 @@
   <si>
     <t xml:space="preserve"># (# on the first column means that the whole row is ignored)
 DO NOT SWAP COLUMNS!</t>
+  </si>
+  <si>
+    <t>42</t>
   </si>
 </sst>
 </file>
@@ -340,7 +345,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="0" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -348,12 +353,12 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.47"/>
+    <col collapsed="false" customWidth="1" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -361,18 +366,132 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11">
+      <c r="C11">
+        <f>=4+3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12">
+        <f>=4+3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25">
+        <f>=4+3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35"/>
+      <c r="Z35"/>
+    </row>
+    <row r="1048576"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -476,6 +595,30 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -483,7 +626,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="0" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -533,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="0" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reworked XLCellIterator (--performance) to not create cells until iterator is dereferenced, created stub for worksheet comments support
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Worksheet name test" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="15" r:id="rId18"/>
+    <sheet state="visible" name="Sheet3" sheetId="15" r:id="rId18"/>
     <sheet name="ChangeLog" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Containers" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Parameters" sheetId="4" state="visible" r:id="rId6"/>
@@ -487,10 +487,39 @@
         <v>0</v>
       </c>
     </row>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
     <row r="35">
       <c r="A35"/>
       <c r="Z35"/>
     </row>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
     <row r="1048576"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -611,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="" workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
2024-09-02 ensure that all worksheets are contained in app.xml <TitlesOfParts> and reflected in <HeadingPairs> value for Worksheets
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet name test" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="2" state="veryHidden" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,15 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="2">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
     <t xml:space="preserve">document version</t>
-  </si>
-  <si>
-    <t>42</t>
   </si>
 </sst>
 </file>
@@ -319,7 +316,7 @@
   </sheetPr>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="0" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -327,7 +324,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.6"/>
-    <col collapsed="false" customWidth="1" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,10 +337,6 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="b">
@@ -376,34 +369,34 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="A3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="0" t="n">
         <v>9</v>
       </c>
     </row>
@@ -417,27 +410,17 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-    </row>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
+    </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="1">
-        <f aca="false">=4+3</f>
-        <v>0</v>
+      <c r="C11" s="1" t="n">
+        <f aca="false">4+3</f>
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="1">
-        <f aca="false">=4+3</f>
-        <v>0</v>
+      <c r="D12" s="4" t="n">
+        <f aca="false">4+3</f>
+        <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,57 +428,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1">
-        <f aca="false">=4+3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35">
-      <c r="A35" s="1"/>
-      <c r="Z35"/>
-    </row>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="1048576"/>
+      <c r="A25" s="1" t="n">
+        <f aca="false">4+3</f>
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -514,7 +452,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="0" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -531,13 +469,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>